<commit_message>
Updated disease pathways 6 extra pathways
</commit_message>
<xml_diff>
--- a/Code/Data/pathway disease filtering.xlsx
+++ b/Code/Data/pathway disease filtering.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.catala\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.catala\Desktop\20220909 Working scripts quantile normalization after homology mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="All pathways more than 10 genes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="594">
   <si>
     <t>pathway</t>
   </si>
@@ -2134,8 +2134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I587"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A572" workbookViewId="0">
-      <selection activeCell="B588" sqref="B588"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117:B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4954,10 +4954,10 @@
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A98">
+      <c r="A98" s="2">
         <v>124</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="2" t="s">
         <v>104</v>
       </c>
       <c r="C98" s="1">
@@ -5505,10 +5505,10 @@
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A117">
+      <c r="A117" s="2">
         <v>153</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C117">
@@ -6259,10 +6259,10 @@
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A143">
+      <c r="A143" s="2">
         <v>185</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C143">
@@ -7274,10 +7274,10 @@
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A178">
+      <c r="A178" s="2">
         <v>224</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C178" s="1">
@@ -17627,10 +17627,10 @@
       </c>
     </row>
     <row r="535" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A535">
+      <c r="A535" s="2">
         <v>670</v>
       </c>
-      <c r="B535" t="s">
+      <c r="B535" s="2" t="s">
         <v>541</v>
       </c>
       <c r="C535" s="1">
@@ -18874,10 +18874,10 @@
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A578">
+      <c r="A578" s="2">
         <v>721</v>
       </c>
-      <c r="B578" t="s">
+      <c r="B578" s="2" t="s">
         <v>584</v>
       </c>
       <c r="C578" s="1">
@@ -19170,10 +19170,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B95"/>
+  <dimension ref="A2:B101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19933,6 +19933,54 @@
         <v>588</v>
       </c>
     </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" s="2">
+        <v>224</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" s="2">
+        <v>721</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" s="2">
+        <v>185</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" s="2">
+        <v>670</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" s="2">
+        <v>124</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" s="2">
+        <v>153</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>